<commit_message>
started to make some changes
</commit_message>
<xml_diff>
--- a/test_registrering/excel/test.xlsx
+++ b/test_registrering/excel/test.xlsx
@@ -403,7 +403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -590,6 +590,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>27.01.2021</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>REA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Everything good. Next step implement input terminal
</commit_message>
<xml_diff>
--- a/test_registrering/excel/test.xlsx
+++ b/test_registrering/excel/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\test_registrering\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4D2E3C-4ACD-4F81-9D6F-DDD8A1B4570F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D964B9C2-D115-4AAB-BDBA-62D298E077AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30870" yWindow="3555" windowWidth="14400" windowHeight="7815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2170" yWindow="1780" windowWidth="14420" windowHeight="7820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hour_register" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Anna</t>
   </si>
@@ -176,9 +176,6 @@
     <t>MVA</t>
   </si>
   <si>
-    <t>MVA-pris</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
@@ -186,6 +183,12 @@
   </si>
   <si>
     <t>Undervising</t>
+  </si>
+  <si>
+    <t>MVA_cost</t>
+  </si>
+  <si>
+    <t>Kundenummer</t>
   </si>
 </sst>
 </file>
@@ -781,7 +784,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -806,21 +809,21 @@
         <v>38</v>
       </c>
       <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" cm="1">
         <f t="array" ref="B2">SUMPRODUCT((MONTH(hour_register!$C$2:$C$1001)=MONTH(1))*(hour_register!$B$2:$B$1001))</f>
@@ -849,6 +852,10 @@
       </c>
       <c r="I2" s="3">
         <v>44228</v>
+      </c>
+      <c r="J2">
+        <f>H2</f>
+        <v>3465</v>
       </c>
     </row>
   </sheetData>
@@ -860,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E101A67-FF19-4B49-BCE2-732349B93EA3}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -886,21 +893,21 @@
         <v>38</v>
       </c>
       <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" cm="1">
         <f t="array" ref="B2">SUMPRODUCT((MONTH(hour_register!$C$2:$C$1001)=MONTH(hour_register!C2&amp;2))*(hour_register!$B$2:$B$1001))</f>
@@ -929,6 +936,10 @@
       </c>
       <c r="I2" s="3">
         <v>44228</v>
+      </c>
+      <c r="J2" s="2">
+        <f>H2</f>
+        <v>3465</v>
       </c>
     </row>
   </sheetData>
@@ -983,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF65E71A-106C-4596-A5DD-DB20503D05E9}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -994,6 +1005,7 @@
     <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1012,7 +1024,9 @@
       <c r="F1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
@@ -1029,6 +1043,10 @@
       </c>
       <c r="E2" t="s">
         <v>21</v>
+      </c>
+      <c r="G2">
+        <f>A2+1</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>